<commit_message>
models update by prakash
</commit_message>
<xml_diff>
--- a/StudentDegreePlan.xlsx
+++ b/StudentDegreePlan.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S534148\Documents\44663\StudentDegreePlan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s533725\Documents\44663\StudentDegreePlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="92">
   <si>
     <t>NumberOfTerms</t>
   </si>
@@ -296,9 +296,6 @@
     <t>StudentID</t>
   </si>
   <si>
-    <t>DegereePlanAbv</t>
-  </si>
-  <si>
     <t>SlotID</t>
   </si>
   <si>
@@ -306,6 +303,9 @@
   </si>
   <si>
     <t>String</t>
+  </si>
+  <si>
+    <t>DegreePlanAbv</t>
   </si>
 </sst>
 </file>
@@ -1724,7 +1724,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1745,7 +1745,7 @@
         <v>87</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D1" s="22" t="s">
         <v>18</v>
@@ -1754,7 +1754,7 @@
         <v>83</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1775,7 +1775,7 @@
       </c>
       <c r="F2" t="str">
         <f>"new DegreePlan{"&amp;$A$1&amp;"="&amp;A2&amp;$B$1&amp;"="&amp;B2&amp;$C$1&amp;"="&amp;C2&amp;$D$1&amp;"="&amp;D2&amp;$E$1&amp;"="&amp;E2&amp;"}"</f>
-        <v>new DegreePlan{DegreePlanID=7251StudentID=533725DegereePlanAbv=Slow and easyDegreePlanName=Take a break in summerDegreeID=1}</v>
+        <v>new DegreePlan{DegreePlanID=7251StudentID=533725DegreePlanAbv=Slow and easyDegreePlanName=Take a break in summerDegreeID=1}</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1796,15 +1796,15 @@
       </c>
       <c r="F3" s="17" t="str">
         <f t="shared" ref="F3:F7" si="0">"new DegreePlan{"&amp;$A$1&amp;"="&amp;A3&amp;$B$1&amp;"="&amp;B3&amp;$C$1&amp;"="&amp;C3&amp;$D$1&amp;"="&amp;D3&amp;$E$1&amp;"="&amp;E3&amp;"}"</f>
-        <v>new DegreePlan{DegreePlanID=7252StudentID=533725DegereePlanAbv=Super FastDegreePlanName=No breakDegreeID=1}</v>
+        <v>new DegreePlan{DegreePlanID=7252StudentID=533725DegreePlanAbv=Super FastDegreePlanName=No breakDegreeID=1}</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="17">
         <v>7253</v>
       </c>
-      <c r="B4" s="20" t="s">
-        <v>21</v>
+      <c r="B4" s="20">
+        <v>534049</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>20</v>
@@ -1817,7 +1817,7 @@
       </c>
       <c r="F4" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreePlan{DegreePlanID=7253StudentID=S534049DegereePlanAbv=Slow and easyDegreePlanName=As fast as I CanDegreeID=1}</v>
+        <v>new DegreePlan{DegreePlanID=7253StudentID=534049DegreePlanAbv=Slow and easyDegreePlanName=As fast as I CanDegreeID=1}</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1838,7 +1838,7 @@
       </c>
       <c r="F5" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreePlan{DegreePlanID=7254StudentID=534049DegereePlanAbv=Slow and easyDegreePlanName=Take less courses per semesterDegreeID=1}</v>
+        <v>new DegreePlan{DegreePlanID=7254StudentID=534049DegreePlanAbv=Slow and easyDegreePlanName=Take less courses per semesterDegreeID=1}</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1859,7 +1859,7 @@
       </c>
       <c r="F6" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreePlan{DegreePlanID=7255StudentID=533767DegereePlanAbv=Super FastDegreePlanName=More subjects in semestersDegreeID=1}</v>
+        <v>new DegreePlan{DegreePlanID=7255StudentID=533767DegreePlanAbv=Super FastDegreePlanName=More subjects in semestersDegreeID=1}</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1880,7 +1880,7 @@
       </c>
       <c r="F7" s="17" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreePlan{DegreePlanID=7256StudentID=533767DegereePlanAbv=Slow and ConsistentDegreePlanName=Take a break in summerDegreeID=1}</v>
+        <v>new DegreePlan{DegreePlanID=7256StudentID=533767DegreePlanAbv=Slow and ConsistentDegreePlanName=Take a break in summerDegreeID=1}</v>
       </c>
     </row>
   </sheetData>
@@ -1892,7 +1892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -2015,7 +2015,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B1" s="28" t="s">
         <v>86</v>
@@ -2393,7 +2393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -2412,7 +2412,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B1" s="23" t="s">
         <v>87</v>

</xml_diff>